<commit_message>
manage bulk param in product CSV import
</commit_message>
<xml_diff>
--- a/www/produitsPro.xlsx
+++ b/www/produitsPro.xlsx
@@ -34,6 +34,7 @@
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="0"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">si le produit est bio, mettre "1" dans la case, sinon laisser vide
 	-François Barbut</t>
@@ -48,9 +49,9 @@
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="0"/>
+            <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Si les clients peuvent commander des quantités à virgule ( par exemple "0,5 poulet" ) , mettre "1" dans la case, sinon laisser vide.
-	-François Barbut</t>
+          <t xml:space="preserve">Mettre 1 si ce produit est vendu en vrac ( pas de contenant, quantité variable )</t>
         </r>
       </text>
     </comment>
@@ -62,6 +63,7 @@
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="0"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">remplir cette case que si nécéssaire de préciser qqe chose par rapport à cette offre ( on a déjà le nom du produit + quantité + unité )
 	-François Barbut</t>
@@ -76,6 +78,7 @@
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="0"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Au format AAAA-MM-JJ , par exemple 2021-02-28</t>
         </r>
@@ -86,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="41">
   <si>
     <t xml:space="preserve">PRODUITS</t>
   </si>
@@ -112,88 +115,91 @@
     <t xml:space="preserve">Bio</t>
   </si>
   <si>
+    <t xml:space="preserve">vrac</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Catégorie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nom offre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quantité ( dans l'unité définie colonne D )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prix H.T</t>
+  </si>
+  <si>
+    <t xml:space="preserve">taux de TVA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">actif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">URL Image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date Image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pommes de Terre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pommes de terre Bintje cultivée en agriculture biologique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PDT-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ici on a définit une offre "Pommes de terre 1kg" à 1,75€</t>
+  </si>
+  <si>
+    <t xml:space="preserve">caisse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PDT-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ici on a définit une offre "Pommes de terre (caisse) 5kg" à 8,75€</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sac</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PDT-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oeufs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OEU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oeufs bio frais de chez Patrick Legrand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">piece</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OEU-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ici on a définit une offre "Oeufs - 6 pièces" à 2€</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OEU-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OEU-8</t>
+  </si>
+  <si>
     <t xml:space="preserve">Quantités "à virgule"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Catégorie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nom offre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quantité ( dans l'unité définie colonne D )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prix H.T</t>
-  </si>
-  <si>
-    <t xml:space="preserve">taux de TVA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">actif</t>
-  </si>
-  <si>
-    <t xml:space="preserve">URL Image</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date Image</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pommes de Terre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PDT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pommes de terre Bintje cultivée en agriculture biologique</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PDT-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ici on a définit une offre "Pommes de terre 1kg" à 1,75€</t>
-  </si>
-  <si>
-    <t xml:space="preserve">caisse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PDT-5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ici on a définit une offre "Pommes de terre (caisse) 5kg" à 8,75€</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sac</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PDT-10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oeufs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OEU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oeufs bio frais de chez Patrick Legrand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">piece</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OEU-2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ici on a définit une offre "Oeufs - 6 pièces" à 2€</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OEU-4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OEU-8</t>
   </si>
   <si>
     <t xml:space="preserve">NB : Après import dans Cagette Pro, il faudra encore catégoriser le produit et ajouter une photo.</t>
@@ -215,12 +221,13 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -234,83 +241,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="24"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="10"/>
-      <color rgb="FF0000EE"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="0"/>
     </font>
@@ -347,11 +277,13 @@
       <sz val="11"/>
       <name val="Cambria"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Cambria"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -359,9 +291,10 @@
       <color rgb="FF666666"/>
       <name val="Cambria"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -370,60 +303,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFFFCCCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFB6D7A8"/>
-        <bgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFCCCCFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFE599"/>
-        <bgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFFFFF99"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -431,23 +322,8 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -471,247 +347,179 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="23">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="En-tête" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Hyperlink" xfId="26" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Status" xfId="27" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Good" xfId="28" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Neutral" xfId="29" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Bad" xfId="30" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Warning" xfId="31" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Error" xfId="32" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent" xfId="33" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 1" xfId="34" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 2" xfId="35" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 3" xfId="36" builtinId="53" customBuiltin="true"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000EE"/>
+      <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFB6D7A8"/>
@@ -723,7 +531,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -735,11 +543,11 @@
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFE599"/>
+      <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FFFFE599"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -762,30 +570,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AG9"/>
+  <dimension ref="A1:AG1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
+      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="23.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="13.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="8.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="6" style="1" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="8.41"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="6" style="1" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="28.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="11.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="16.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="16.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="16.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="54.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="17" style="1" width="14.43"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="17" style="1" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -893,7 +701,9 @@
       <c r="E3" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="F3" s="14"/>
+      <c r="F3" s="14" t="n">
+        <v>0</v>
+      </c>
       <c r="G3" s="14"/>
       <c r="H3" s="12"/>
       <c r="I3" s="12" t="s">
@@ -1008,7 +818,9 @@
       <c r="E6" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="F6" s="14"/>
+      <c r="F6" s="14" t="n">
+        <v>0</v>
+      </c>
       <c r="G6" s="14"/>
       <c r="H6" s="12"/>
       <c r="I6" s="12" t="s">
@@ -2106,26 +1918,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:AC1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="5" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="14.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="54.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2165,7 +1974,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="23" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="G2" s="24" t="s">
         <v>10</v>
@@ -2183,7 +1992,7 @@
         <v>13</v>
       </c>
       <c r="L2" s="26" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="M2" s="27"/>
       <c r="N2" s="27"/>
@@ -2407,14 +2216,14 @@
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="36" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B11" s="35" t="s">
         <v>29</v>
       </c>
       <c r="C11" s="35"/>
       <c r="D11" s="34" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E11" s="34" t="n">
         <v>1</v>
@@ -2422,7 +2231,7 @@
       <c r="F11" s="34"/>
       <c r="G11" s="35"/>
       <c r="H11" s="35" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I11" s="34" t="n">
         <v>6</v>

</xml_diff>